<commit_message>
commit before change name repository xlsx
</commit_message>
<xml_diff>
--- a/EuroDreams_Stat.xlsx
+++ b/EuroDreams_Stat.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="16">
   <si>
     <t>Numéros</t>
   </si>
@@ -25,85 +25,43 @@
     <t>Dernière sortie</t>
   </si>
   <si>
-    <t>8.82</t>
-  </si>
-  <si>
-    <t>29.41</t>
-  </si>
-  <si>
-    <t>20.59</t>
-  </si>
-  <si>
-    <t>5.88</t>
-  </si>
-  <si>
-    <t>14.71</t>
-  </si>
-  <si>
-    <t>11.76</t>
-  </si>
-  <si>
-    <t>17.65</t>
-  </si>
-  <si>
-    <t>23.53</t>
-  </si>
-  <si>
-    <t>26.47</t>
-  </si>
-  <si>
-    <t>2.94</t>
-  </si>
-  <si>
-    <t>25/01/24</t>
-  </si>
-  <si>
-    <t>26/02/24</t>
-  </si>
-  <si>
-    <t>15/02/24</t>
-  </si>
-  <si>
-    <t>12/02/24</t>
-  </si>
-  <si>
-    <t>19/02/24</t>
-  </si>
-  <si>
-    <t>22/02/24</t>
-  </si>
-  <si>
-    <t>29/02/24</t>
-  </si>
-  <si>
-    <t>01/02/24</t>
-  </si>
-  <si>
-    <t>08/01/24</t>
-  </si>
-  <si>
-    <t>25/12/23</t>
-  </si>
-  <si>
-    <t>01/01/24</t>
-  </si>
-  <si>
-    <t>08/02/24</t>
-  </si>
-  <si>
-    <t>29/01/24</t>
-  </si>
-  <si>
-    <t>18/01/24</t>
-  </si>
-  <si>
-    <t>11/12/23</t>
-  </si>
-  <si>
-    <t>22/01/24</t>
-  </si>
-  <si>
     <t>Pourcentage de sorties</t>
+  </si>
+  <si>
+    <t>9.76</t>
+  </si>
+  <si>
+    <t>26.83</t>
+  </si>
+  <si>
+    <t>24.39</t>
+  </si>
+  <si>
+    <t>4.88</t>
+  </si>
+  <si>
+    <t>17.07</t>
+  </si>
+  <si>
+    <t>14.63</t>
+  </si>
+  <si>
+    <t>7.32</t>
+  </si>
+  <si>
+    <t>21.95</t>
+  </si>
+  <si>
+    <t>12.20</t>
+  </si>
+  <si>
+    <t>19.51</t>
+  </si>
+  <si>
+    <t>2.44</t>
+  </si>
+  <si>
+    <t>29.27</t>
   </si>
 </sst>
 </file>
@@ -158,7 +116,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -170,6 +128,12 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -466,8 +430,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="A42" sqref="A42:D46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
@@ -483,7 +447,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>29</v>
+        <v>3</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>2</v>
@@ -494,13 +458,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="2">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>13</v>
+        <v>4</v>
+      </c>
+      <c r="D2" s="5">
+        <v>45355</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -508,13 +472,13 @@
         <v>2</v>
       </c>
       <c r="B3" s="3">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>14</v>
+        <v>5</v>
+      </c>
+      <c r="D3" s="6">
+        <v>45362</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -522,13 +486,13 @@
         <v>3</v>
       </c>
       <c r="B4" s="2">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>15</v>
+        <v>6</v>
+      </c>
+      <c r="D4" s="5">
+        <v>45376</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -539,10 +503,10 @@
         <v>2</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>16</v>
+        <v>7</v>
+      </c>
+      <c r="D5" s="6">
+        <v>45334</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -553,10 +517,10 @@
         <v>7</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>15</v>
+        <v>8</v>
+      </c>
+      <c r="D6" s="5">
+        <v>45337</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -564,13 +528,13 @@
         <v>6</v>
       </c>
       <c r="B7" s="3">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>16</v>
+        <v>9</v>
+      </c>
+      <c r="D7" s="6">
+        <v>45369</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -578,13 +542,13 @@
         <v>7</v>
       </c>
       <c r="B8" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>17</v>
+        <v>10</v>
+      </c>
+      <c r="D8" s="5">
+        <v>45362</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -592,13 +556,13 @@
         <v>8</v>
       </c>
       <c r="B9" s="3">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>18</v>
+        <v>11</v>
+      </c>
+      <c r="D9" s="6">
+        <v>45372</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -609,10 +573,10 @@
         <v>3</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>16</v>
+        <v>10</v>
+      </c>
+      <c r="D10" s="5">
+        <v>45334</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -620,13 +584,13 @@
         <v>10</v>
       </c>
       <c r="B11" s="3">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>19</v>
+        <v>9</v>
+      </c>
+      <c r="D11" s="6">
+        <v>45355</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -637,10 +601,10 @@
         <v>4</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D12" s="4" t="s">
-        <v>19</v>
+        <v>4</v>
+      </c>
+      <c r="D12" s="5">
+        <v>45351</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -648,13 +612,13 @@
         <v>12</v>
       </c>
       <c r="B13" s="3">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D13" s="4" t="s">
-        <v>20</v>
+        <v>12</v>
+      </c>
+      <c r="D13" s="6">
+        <v>45376</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -662,13 +626,13 @@
         <v>13</v>
       </c>
       <c r="B14" s="2">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D14" s="4" t="s">
-        <v>21</v>
+        <v>8</v>
+      </c>
+      <c r="D14" s="5">
+        <v>45365</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -676,13 +640,13 @@
         <v>14</v>
       </c>
       <c r="B15" s="3">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D15" s="4" t="s">
-        <v>15</v>
+        <v>12</v>
+      </c>
+      <c r="D15" s="6">
+        <v>45362</v>
       </c>
     </row>
     <row r="16" spans="1:4">
@@ -690,13 +654,13 @@
         <v>15</v>
       </c>
       <c r="B16" s="2">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D16" s="4" t="s">
-        <v>14</v>
+        <v>11</v>
+      </c>
+      <c r="D16" s="5">
+        <v>45376</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -709,8 +673,8 @@
       <c r="C17" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D17" s="4" t="s">
-        <v>15</v>
+      <c r="D17" s="6">
+        <v>45337</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -721,10 +685,10 @@
         <v>2</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D18" s="4" t="s">
-        <v>22</v>
+        <v>7</v>
+      </c>
+      <c r="D18" s="5">
+        <v>45285</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -732,13 +696,13 @@
         <v>18</v>
       </c>
       <c r="B19" s="3">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D19" s="4" t="s">
-        <v>23</v>
+        <v>9</v>
+      </c>
+      <c r="D19" s="6">
+        <v>45369</v>
       </c>
     </row>
     <row r="20" spans="1:4">
@@ -746,13 +710,13 @@
         <v>19</v>
       </c>
       <c r="B20" s="2">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D20" s="4" t="s">
-        <v>14</v>
+        <v>8</v>
+      </c>
+      <c r="D20" s="5">
+        <v>45369</v>
       </c>
     </row>
     <row r="21" spans="1:4">
@@ -760,13 +724,13 @@
         <v>20</v>
       </c>
       <c r="B21" s="3">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D21" s="4" t="s">
-        <v>18</v>
+        <v>12</v>
+      </c>
+      <c r="D21" s="6">
+        <v>45376</v>
       </c>
     </row>
     <row r="22" spans="1:4">
@@ -777,10 +741,10 @@
         <v>8</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D22" s="4" t="s">
-        <v>19</v>
+        <v>13</v>
+      </c>
+      <c r="D22" s="5">
+        <v>45351</v>
       </c>
     </row>
     <row r="23" spans="1:4">
@@ -788,13 +752,13 @@
         <v>22</v>
       </c>
       <c r="B23" s="3">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D23" s="4" t="s">
-        <v>24</v>
+        <v>8</v>
+      </c>
+      <c r="D23" s="6">
+        <v>45362</v>
       </c>
     </row>
     <row r="24" spans="1:4">
@@ -802,13 +766,13 @@
         <v>23</v>
       </c>
       <c r="B24" s="2">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D24" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
+      </c>
+      <c r="D24" s="5">
+        <v>45358</v>
       </c>
     </row>
     <row r="25" spans="1:4">
@@ -816,13 +780,13 @@
         <v>24</v>
       </c>
       <c r="B25" s="3">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D25" s="4" t="s">
-        <v>18</v>
+        <v>9</v>
+      </c>
+      <c r="D25" s="6">
+        <v>45369</v>
       </c>
     </row>
     <row r="26" spans="1:4">
@@ -830,13 +794,13 @@
         <v>25</v>
       </c>
       <c r="B26" s="2">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D26" s="4" t="s">
-        <v>17</v>
+        <v>5</v>
+      </c>
+      <c r="D26" s="5">
+        <v>45376</v>
       </c>
     </row>
     <row r="27" spans="1:4">
@@ -849,8 +813,8 @@
       <c r="C27" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D27" s="4" t="s">
-        <v>24</v>
+      <c r="D27" s="6">
+        <v>45330</v>
       </c>
     </row>
     <row r="28" spans="1:4">
@@ -858,13 +822,13 @@
         <v>27</v>
       </c>
       <c r="B28" s="2">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D28" s="4" t="s">
-        <v>25</v>
+        <v>13</v>
+      </c>
+      <c r="D28" s="5">
+        <v>45376</v>
       </c>
     </row>
     <row r="29" spans="1:4">
@@ -875,10 +839,10 @@
         <v>4</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D29" s="4" t="s">
-        <v>20</v>
+        <v>4</v>
+      </c>
+      <c r="D29" s="6">
+        <v>45323</v>
       </c>
     </row>
     <row r="30" spans="1:4">
@@ -886,13 +850,13 @@
         <v>29</v>
       </c>
       <c r="B30" s="2">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D30" s="4" t="s">
-        <v>25</v>
+        <v>13</v>
+      </c>
+      <c r="D30" s="5">
+        <v>45355</v>
       </c>
     </row>
     <row r="31" spans="1:4">
@@ -900,13 +864,13 @@
         <v>30</v>
       </c>
       <c r="B31" s="3">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D31" s="4" t="s">
-        <v>26</v>
+        <v>9</v>
+      </c>
+      <c r="D31" s="6">
+        <v>45372</v>
       </c>
     </row>
     <row r="32" spans="1:4">
@@ -914,13 +878,13 @@
         <v>31</v>
       </c>
       <c r="B32" s="2">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D32" s="4" t="s">
-        <v>19</v>
+        <v>12</v>
+      </c>
+      <c r="D32" s="5">
+        <v>45358</v>
       </c>
     </row>
     <row r="33" spans="1:5">
@@ -931,10 +895,10 @@
         <v>5</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D33" s="4" t="s">
-        <v>27</v>
+        <v>12</v>
+      </c>
+      <c r="D33" s="6">
+        <v>45271</v>
       </c>
     </row>
     <row r="34" spans="1:5">
@@ -942,13 +906,13 @@
         <v>33</v>
       </c>
       <c r="B34" s="2">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D34" s="4" t="s">
-        <v>20</v>
+        <v>13</v>
+      </c>
+      <c r="D34" s="5">
+        <v>45372</v>
       </c>
     </row>
     <row r="35" spans="1:5">
@@ -959,10 +923,10 @@
         <v>1</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D35" s="4" t="s">
-        <v>28</v>
+        <v>14</v>
+      </c>
+      <c r="D35" s="6">
+        <v>45313</v>
       </c>
     </row>
     <row r="36" spans="1:5">
@@ -970,13 +934,13 @@
         <v>35</v>
       </c>
       <c r="B36" s="2">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D36" s="4" t="s">
-        <v>20</v>
+        <v>11</v>
+      </c>
+      <c r="D36" s="5">
+        <v>45365</v>
       </c>
     </row>
     <row r="37" spans="1:5">
@@ -987,10 +951,10 @@
         <v>2</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D37" s="4" t="s">
-        <v>24</v>
+        <v>7</v>
+      </c>
+      <c r="D37" s="6">
+        <v>45330</v>
       </c>
     </row>
     <row r="38" spans="1:5">
@@ -998,13 +962,13 @@
         <v>37</v>
       </c>
       <c r="B38" s="2">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D38" s="4" t="s">
-        <v>14</v>
+        <v>9</v>
+      </c>
+      <c r="D38" s="5">
+        <v>45372</v>
       </c>
     </row>
     <row r="39" spans="1:5">
@@ -1015,10 +979,10 @@
         <v>5</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D39" s="4" t="s">
-        <v>19</v>
+        <v>12</v>
+      </c>
+      <c r="D39" s="6">
+        <v>45351</v>
       </c>
     </row>
     <row r="40" spans="1:5">
@@ -1026,13 +990,13 @@
         <v>39</v>
       </c>
       <c r="B40" s="2">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D40" s="4" t="s">
-        <v>18</v>
+        <v>13</v>
+      </c>
+      <c r="D40" s="5">
+        <v>45369</v>
       </c>
     </row>
     <row r="41" spans="1:5">
@@ -1043,10 +1007,10 @@
         <v>8</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D41" s="4" t="s">
-        <v>19</v>
+        <v>13</v>
+      </c>
+      <c r="D41" s="6">
+        <v>45351</v>
       </c>
     </row>
     <row r="42" spans="1:5">
@@ -1054,13 +1018,13 @@
         <v>1</v>
       </c>
       <c r="B42" s="2">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D42" s="4" t="s">
-        <v>19</v>
+        <v>15</v>
+      </c>
+      <c r="D42" s="5">
+        <v>45362</v>
       </c>
       <c r="E42" s="4"/>
     </row>
@@ -1069,13 +1033,13 @@
         <v>2</v>
       </c>
       <c r="B43" s="3">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D43" s="4" t="s">
-        <v>14</v>
+        <v>8</v>
+      </c>
+      <c r="D43" s="6">
+        <v>45372</v>
       </c>
       <c r="E43" s="4"/>
     </row>
@@ -1084,13 +1048,13 @@
         <v>3</v>
       </c>
       <c r="B44" s="2">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D44" s="4" t="s">
-        <v>20</v>
+        <v>12</v>
+      </c>
+      <c r="D44" s="5">
+        <v>45376</v>
       </c>
       <c r="E44" s="4"/>
     </row>
@@ -1102,10 +1066,10 @@
         <v>8</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D45" s="4" t="s">
-        <v>18</v>
+        <v>13</v>
+      </c>
+      <c r="D45" s="6">
+        <v>45344</v>
       </c>
       <c r="E45" s="4"/>
     </row>
@@ -1119,8 +1083,8 @@
       <c r="C46" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D46" s="4" t="s">
-        <v>26</v>
+      <c r="D46" s="5">
+        <v>45309</v>
       </c>
       <c r="E46" s="4"/>
     </row>

</xml_diff>